<commit_message>
Updated Hawaii Case Filing Juvenile information
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/hawaii/CaseFiling.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/hawaii/CaseFiling.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="600" windowWidth="27300" windowHeight="13740"/>
+    <workbookView xWindow="5500" yWindow="1720" windowWidth="27300" windowHeight="13740"/>
   </bookViews>
   <sheets>
-    <sheet name="Prosecution Case Filing" sheetId="1" r:id="rId1"/>
+    <sheet name="Case Filing Decision" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -1017,9 +1017,6 @@
     <t>Hawaii Term</t>
   </si>
   <si>
-    <t>Hawaii PA Document</t>
-  </si>
-  <si>
     <t>Citizenship</t>
   </si>
   <si>
@@ -1504,13 +1501,16 @@
   </si>
   <si>
     <t>Employee Occupation Text</t>
+  </si>
+  <si>
+    <t>Hawaii PA Document (JJIS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1683,6 +1683,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1779,7 +1786,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="421">
+  <cellStyleXfs count="439">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2201,8 +2208,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2321,8 +2346,11 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="421">
+  <cellStyles count="439">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2547,6 +2575,15 @@
     <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2738,6 +2775,15 @@
     <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="90"/>
@@ -3044,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3061,7 +3107,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="49" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>331</v>
+        <v>493</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>330</v>
@@ -3094,7 +3140,7 @@
         <v>72</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3105,7 +3151,7 @@
         <v>72</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3116,10 +3162,10 @@
         <v>72</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3127,7 +3173,7 @@
         <v>71</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3138,7 +3184,7 @@
         <v>61</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3207,7 +3253,7 @@
         <v>116</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="42">
@@ -3224,7 +3270,7 @@
         <v>121</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="42">
@@ -3241,10 +3287,10 @@
         <v>117</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="42">
       <c r="D15" s="7" t="s">
         <v>28</v>
       </c>
@@ -3252,10 +3298,10 @@
         <v>116</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3309,7 @@
         <v>118</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="42">
@@ -3274,7 +3320,7 @@
         <v>116</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="98">
@@ -3285,10 +3331,10 @@
         <v>119</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="13"/>
@@ -3299,7 +3345,7 @@
         <v>120</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3322,7 +3368,7 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3345,10 +3391,10 @@
         <v>166</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="13"/>
@@ -3359,12 +3405,12 @@
         <v>113</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A25" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="13"/>
@@ -3375,7 +3421,7 @@
         <v>122</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3396,7 +3442,7 @@
         <v>74</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="28">
@@ -3414,7 +3460,7 @@
         <v>66</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1" ht="42">
@@ -3428,10 +3474,10 @@
         <v>88</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="13"/>
@@ -3442,7 +3488,7 @@
         <v>154</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1">
@@ -3473,7 +3519,7 @@
       <c r="E32" s="23"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="33" spans="1:6" s="2" customFormat="1">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
         <v>202</v>
@@ -3488,7 +3534,7 @@
         <v>201</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" ht="28">
@@ -3506,10 +3552,10 @@
         <v>85</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
         <v>125</v>
@@ -3524,10 +3570,10 @@
         <v>86</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
         <v>195</v>
@@ -3542,10 +3588,10 @@
         <v>87</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" ht="28">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
         <v>196</v>
@@ -3560,7 +3606,7 @@
         <v>173</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1">
@@ -3578,7 +3624,7 @@
         <v>173</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1">
@@ -3596,7 +3642,7 @@
         <v>199</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1">
@@ -3614,174 +3660,174 @@
         <v>159</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="D41" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>368</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>369</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1">
       <c r="A47" s="38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="26"/>
       <c r="D47" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="12"/>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1">
       <c r="A48" s="38" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="26"/>
       <c r="D48" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1">
       <c r="A49" s="38" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="26"/>
       <c r="D49" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="12"/>
     </row>
     <row r="50" spans="1:6" s="2" customFormat="1">
       <c r="A50" s="38" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="26"/>
       <c r="D50" s="36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="12"/>
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1">
       <c r="A51" s="38" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="26"/>
       <c r="D51" s="36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="12"/>
     </row>
     <row r="52" spans="1:6" s="2" customFormat="1">
       <c r="A52" s="38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="26"/>
       <c r="D52" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="12"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="7"/>
@@ -3794,7 +3840,7 @@
       <c r="E57" s="15"/>
       <c r="F57" s="30"/>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="58" spans="1:6" s="2" customFormat="1">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="13"/>
@@ -3805,7 +3851,7 @@
         <v>10</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="2" customFormat="1">
@@ -3850,7 +3896,7 @@
         <v>188</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3894,10 +3940,10 @@
         <v>194</v>
       </c>
       <c r="F65" s="31" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="2" customFormat="1" ht="28">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="2" customFormat="1">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="13"/>
@@ -3908,10 +3954,10 @@
         <v>75</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="2" customFormat="1" ht="28">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="2" customFormat="1">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="13"/>
@@ -3922,10 +3968,10 @@
         <v>76</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="2" customFormat="1" ht="28">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="2" customFormat="1" ht="42">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="13"/>
@@ -3936,7 +3982,7 @@
         <v>77</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1" ht="42">
@@ -3954,12 +4000,12 @@
         <v>78</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1" ht="42">
       <c r="A70" s="39" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>237</v>
@@ -3972,7 +4018,7 @@
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="2" customFormat="1">
@@ -4002,12 +4048,12 @@
         <v>68</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="2" customFormat="1">
       <c r="A73" s="38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="26"/>
@@ -4019,7 +4065,7 @@
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1">
       <c r="A74" s="38" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="26"/>
@@ -4040,7 +4086,7 @@
         <v>79</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1" ht="42">
@@ -4054,10 +4100,10 @@
         <v>80</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="2" customFormat="1" ht="28">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="2" customFormat="1">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="13"/>
@@ -4068,12 +4114,12 @@
         <v>81</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1" ht="56">
       <c r="A78" s="39" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B78" s="9"/>
       <c r="C78" s="13"/>
@@ -4084,10 +4130,10 @@
         <v>82</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="2" customFormat="1" ht="28">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="2" customFormat="1" ht="42">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="13"/>
@@ -4098,7 +4144,7 @@
         <v>84</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>83</v>
@@ -4115,7 +4161,7 @@
         <v>113</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4137,7 +4183,7 @@
       </c>
       <c r="E82" s="10"/>
       <c r="F82" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4157,7 +4203,7 @@
         <v>89</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4177,7 +4223,7 @@
         <v>90</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4197,7 +4243,7 @@
         <v>91</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4217,7 +4263,7 @@
         <v>158</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4235,7 +4281,7 @@
       </c>
       <c r="E87" s="22"/>
       <c r="F87" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4255,7 +4301,7 @@
         <v>92</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4269,7 +4315,7 @@
         <v>93</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4283,7 +4329,7 @@
         <v>94</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="2" customFormat="1">
@@ -4313,7 +4359,7 @@
         <v>95</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="2" customFormat="1" ht="56">
@@ -4327,7 +4373,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4345,7 +4391,7 @@
         <v>97</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="2" customFormat="1" ht="56">
@@ -4363,7 +4409,7 @@
         <v>96</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4383,7 +4429,7 @@
         <v>173</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4401,7 +4447,7 @@
         <v>160</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4415,7 +4461,7 @@
         <v>161</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4433,7 +4479,7 @@
         <v>170</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="42">
@@ -4444,7 +4490,7 @@
         <v>171</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="101" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4462,7 +4508,7 @@
         <v>162</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4480,7 +4526,7 @@
         <v>163</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="103" spans="1:6" s="2" customFormat="1" ht="42">
@@ -4500,7 +4546,7 @@
         <v>172</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="42">
@@ -4517,32 +4563,32 @@
         <v>187</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C105" s="25"/>
       <c r="D105" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F105" s="12"/>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="37" t="s">
-        <v>333</v>
+      <c r="A106" s="40" t="s">
+        <v>332</v>
       </c>
       <c r="C106" s="25"/>
       <c r="D106" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F106" s="12"/>
     </row>
     <row r="107" spans="1:6">
       <c r="D107" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E107" s="15"/>
       <c r="F107" s="30"/>
@@ -4552,7 +4598,7 @@
         <v>40</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E108" s="10"/>
       <c r="F108" s="7"/>
@@ -4572,7 +4618,7 @@
         <v>98</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E110" s="10"/>
       <c r="F110" s="7"/>
@@ -4582,7 +4628,7 @@
         <v>324</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E111" s="10"/>
       <c r="F111" s="7"/>
@@ -4608,21 +4654,21 @@
       <c r="F113" s="7"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="37" t="s">
-        <v>344</v>
+      <c r="A114" s="40" t="s">
+        <v>343</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E114" s="10"/>
       <c r="F114" s="7"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="37" t="s">
-        <v>345</v>
+      <c r="A115" s="40" t="s">
+        <v>344</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E115" s="10"/>
       <c r="F115" s="7"/>
@@ -4652,7 +4698,7 @@
       </c>
       <c r="E117" s="22"/>
       <c r="F117" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="118" spans="1:10" s="2" customFormat="1" ht="42">
@@ -4670,7 +4716,7 @@
       </c>
       <c r="E118" s="22"/>
       <c r="F118" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119" spans="1:10" s="2" customFormat="1" ht="42">
@@ -4688,17 +4734,17 @@
       </c>
       <c r="E119" s="22"/>
       <c r="F119" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="120" spans="1:10" s="2" customFormat="1">
       <c r="A120" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B120" s="9"/>
       <c r="C120" s="26"/>
       <c r="D120" s="34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E120" s="22"/>
       <c r="F120" s="12"/>
@@ -4714,7 +4760,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="1:10" ht="28">
+    <row r="122" spans="1:10">
       <c r="B122" s="4" t="s">
         <v>205</v>
       </c>
@@ -4725,10 +4771,10 @@
         <v>206</v>
       </c>
       <c r="F122" s="12" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" s="2" customFormat="1" ht="28">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="2" customFormat="1">
       <c r="A123" s="9"/>
       <c r="B123" s="9" t="s">
         <v>136</v>
@@ -4743,7 +4789,7 @@
         <v>5</v>
       </c>
       <c r="F123" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="124" spans="1:10" s="2" customFormat="1" ht="28">
@@ -4761,7 +4807,7 @@
         <v>71</v>
       </c>
       <c r="F124" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -4775,7 +4821,7 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="1:10" ht="28">
+    <row r="126" spans="1:10" ht="42">
       <c r="D126" s="7" t="s">
         <v>50</v>
       </c>
@@ -4783,7 +4829,7 @@
         <v>175</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
@@ -4819,7 +4865,7 @@
         <v>99</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="130" spans="4:10" ht="42">
@@ -4830,7 +4876,7 @@
         <v>62</v>
       </c>
       <c r="F130" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="131" spans="4:10" ht="42">
@@ -4841,7 +4887,7 @@
         <v>63</v>
       </c>
       <c r="F131" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
@@ -4856,7 +4902,7 @@
         <v>64</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
@@ -4871,7 +4917,7 @@
         <v>114</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
@@ -4886,7 +4932,7 @@
         <v>96</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
@@ -4901,7 +4947,7 @@
         <v>115</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
@@ -4923,7 +4969,7 @@
         <v>99</v>
       </c>
       <c r="F137" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="138" spans="4:10" ht="42">
@@ -4934,7 +4980,7 @@
         <v>101</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="139" spans="4:10" ht="42">
@@ -4945,7 +4991,7 @@
         <v>102</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -4960,7 +5006,7 @@
         <v>103</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
@@ -4975,7 +5021,7 @@
         <v>104</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -4990,14 +5036,14 @@
         <v>105</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
     </row>
-    <row r="143" spans="4:10" ht="28">
+    <row r="143" spans="4:10">
       <c r="D143" s="7" t="s">
         <v>44</v>
       </c>
@@ -5005,7 +5051,7 @@
         <v>106</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -5027,7 +5073,7 @@
         <v>108</v>
       </c>
       <c r="F145" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="42">
@@ -5038,7 +5084,7 @@
         <v>109</v>
       </c>
       <c r="F146" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="147" spans="1:10" ht="42">
@@ -5049,7 +5095,7 @@
         <v>102</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
@@ -5064,7 +5110,7 @@
         <v>110</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
@@ -5079,7 +5125,7 @@
         <v>111</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
@@ -5094,7 +5140,7 @@
         <v>96</v>
       </c>
       <c r="F150" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
@@ -5109,7 +5155,7 @@
         <v>112</v>
       </c>
       <c r="F151" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
@@ -5144,7 +5190,7 @@
         <v>329</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
@@ -5165,7 +5211,7 @@
         <v>71</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
@@ -5186,7 +5232,7 @@
         <v>71</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
@@ -5195,12 +5241,12 @@
     </row>
     <row r="156" spans="1:10">
       <c r="A156" s="37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B156" s="35"/>
       <c r="C156" s="25"/>
       <c r="D156" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E156" s="10"/>
       <c r="F156" s="7"/>
@@ -5211,12 +5257,12 @@
     </row>
     <row r="157" spans="1:10">
       <c r="A157" s="37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B157" s="35"/>
       <c r="C157" s="25"/>
       <c r="D157" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E157" s="10"/>
       <c r="F157" s="7"/>
@@ -5227,12 +5273,12 @@
     </row>
     <row r="158" spans="1:10">
       <c r="A158" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B158" s="35"/>
       <c r="C158" s="25"/>
       <c r="D158" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E158" s="10"/>
       <c r="F158" s="7"/>
@@ -5253,7 +5299,7 @@
         <v>60</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
@@ -5275,7 +5321,7 @@
         <v>180</v>
       </c>
       <c r="F160" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
@@ -5299,7 +5345,7 @@
         <v>183</v>
       </c>
       <c r="F161" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
@@ -5323,7 +5369,7 @@
         <v>184</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
@@ -5347,7 +5393,7 @@
         <v>181</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
@@ -5368,7 +5414,7 @@
         <v>182</v>
       </c>
       <c r="F164" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
@@ -5378,7 +5424,7 @@
     <row r="165" spans="1:10">
       <c r="C165" s="25"/>
       <c r="D165" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E165" s="15"/>
       <c r="F165" s="30"/>
@@ -5389,11 +5435,11 @@
     </row>
     <row r="166" spans="1:10">
       <c r="A166" s="37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C166" s="25"/>
       <c r="D166" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E166" s="10"/>
       <c r="F166" s="7"/>
@@ -5404,11 +5450,11 @@
     </row>
     <row r="167" spans="1:10">
       <c r="A167" s="37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C167" s="25"/>
       <c r="D167" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E167" s="10"/>
       <c r="F167" s="7"/>
@@ -5419,11 +5465,11 @@
     </row>
     <row r="168" spans="1:10">
       <c r="A168" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C168" s="25"/>
       <c r="D168" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E168" s="10"/>
       <c r="F168" s="7"/>
@@ -5479,7 +5525,7 @@
     </row>
     <row r="172" spans="1:10">
       <c r="D172" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E172" s="15"/>
       <c r="F172" s="30"/>
@@ -5503,7 +5549,7 @@
         <v>176</v>
       </c>
       <c r="F173" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="56">
@@ -5523,7 +5569,7 @@
         <v>177</v>
       </c>
       <c r="F174" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
@@ -5533,7 +5579,7 @@
     <row r="175" spans="1:10">
       <c r="C175" s="25"/>
       <c r="D175" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E175" s="5"/>
       <c r="F175" s="12"/>
@@ -5572,7 +5618,7 @@
       <c r="A178" s="33"/>
       <c r="C178" s="25"/>
       <c r="D178" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E178" s="5"/>
       <c r="F178" s="12"/>
@@ -5595,7 +5641,7 @@
         <v>178</v>
       </c>
       <c r="F179" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
@@ -5616,7 +5662,7 @@
         <v>179</v>
       </c>
       <c r="F180" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
@@ -5625,7 +5671,7 @@
     </row>
     <row r="181" spans="1:10">
       <c r="D181" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E181" s="15"/>
       <c r="F181" s="30"/>
@@ -5642,7 +5688,7 @@
         <v>139</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E182" s="10"/>
       <c r="F182" s="7"/>
@@ -5653,13 +5699,13 @@
     </row>
     <row r="183" spans="1:10">
       <c r="A183" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E183" s="10"/>
       <c r="F183" s="7"/>
@@ -5689,7 +5735,7 @@
         <v>186</v>
       </c>
       <c r="F185" s="32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
@@ -5710,7 +5756,7 @@
         <v>185</v>
       </c>
       <c r="F186" s="32" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
@@ -5735,7 +5781,7 @@
         <v>173</v>
       </c>
       <c r="F188" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="42">
@@ -5749,7 +5795,7 @@
         <v>173</v>
       </c>
       <c r="F189" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="42">
@@ -5763,7 +5809,7 @@
         <v>173</v>
       </c>
       <c r="F190" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="191" spans="1:10">

</xml_diff>